<commit_message>
- Klassendiagramme Middlewarelayer erstellen - Webservice Definition erstellen - Example Sequenzdiagramm erstellt - Use Case Diagramm aktualisiert - Designdokument erstellt - Schlaf geraubt
</commit_message>
<xml_diff>
--- a/doku/WI25_Erstellen_Testplan.xlsx
+++ b/doku/WI25_Erstellen_Testplan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaszueger/Desktop/es/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Documents\FFHS\git\ESHH\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1800" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="1800" windowWidth="25605" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -257,8 +257,27 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:H16" totalsRowShown="0">
+  <autoFilter ref="B1:H16"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Zu Testendes Feature"/>
+    <tableColumn id="2" name="Bemerkung"/>
+    <tableColumn id="3" name="Ausgangskriterien"/>
+    <tableColumn id="4" name="zu testende Handlung"/>
+    <tableColumn id="5" name="erwartete Reaktion"/>
+    <tableColumn id="6" name="tatsächliche Reaktion"/>
+    <tableColumn id="7" name="Fazit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,21 +546,21 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.375" customWidth="1"/>
     <col min="5" max="5" width="53.5" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -587,7 +606,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -607,7 +626,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -627,7 +646,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -647,7 +666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -667,7 +686,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -687,7 +706,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -707,7 +726,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -727,7 +746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -747,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -767,7 +786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -787,7 +806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -807,7 +826,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -827,7 +846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -847,7 +866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -869,5 +888,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>